<commit_message>
Add new Acessos File
</commit_message>
<xml_diff>
--- a/Acessos.xlsx
+++ b/Acessos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\unosilva\Documents\Projeto Meli Awards\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E6EA1AD-2038-490B-8E48-0E460D2EB21D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3205E07-BF73-43D6-8D61-8004D5E6B9DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{F6876E12-98B3-4F33-AF0F-22A5C1C00DD2}"/>
   </bookViews>
@@ -17,7 +17,7 @@
     <sheet name="Categorias" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Acessos!$A$1:$C$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Acessos!$A$1:$D$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Categorias!$A$1:$B$334</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="686" uniqueCount="352">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="693" uniqueCount="356">
   <si>
     <t>E-mail</t>
   </si>
@@ -1097,16 +1097,35 @@
   </si>
   <si>
     <t>Teste</t>
+  </si>
+  <si>
+    <t>Teste1</t>
+  </si>
+  <si>
+    <t>Teste2</t>
+  </si>
+  <si>
+    <t>Senha</t>
+  </si>
+  <si>
+    <t>Teste3</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1132,8 +1151,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1468,10 +1488,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2939FEBB-D56D-4D0D-8366-6ACEEBE32804}">
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1479,7 +1499,7 @@
     <col min="1" max="2" width="15.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1489,8 +1509,11 @@
       <c r="C1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D1" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -1498,23 +1521,23 @@
         <v>348</v>
       </c>
       <c r="C2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>346</v>
       </c>
       <c r="B3" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="C3" t="s">
-        <v>319</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>2</v>
+        <v>351</v>
       </c>
       <c r="B4" t="s">
         <v>349</v>
@@ -1523,30 +1546,52 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>2</v>
+        <v>352</v>
       </c>
       <c r="B5" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="C5" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>351</v>
+        <v>353</v>
       </c>
       <c r="B6" t="s">
         <v>349</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>355</v>
+      </c>
+      <c r="B7" t="s">
+        <v>350</v>
+      </c>
+      <c r="C7" t="s">
         <v>3</v>
       </c>
     </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>2</v>
+      </c>
+      <c r="B8" t="s">
+        <v>350</v>
+      </c>
+      <c r="C8" t="s">
+        <v>76</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:C1" xr:uid="{2939FEBB-D56D-4D0D-8366-6ACEEBE32804}"/>
+  <autoFilter ref="A1:D1" xr:uid="{2939FEBB-D56D-4D0D-8366-6ACEEBE32804}"/>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
 </file>
@@ -1555,8 +1600,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{94CC248E-3C21-4DCC-815C-0A279EC017CB}">
   <dimension ref="A1:B334"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+    <sheetView topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="A73" sqref="A73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>